<commit_message>
tweaks to assignment 3 and session 10 slides
</commit_message>
<xml_diff>
--- a/assignments/assign3/params_assign3.xlsx
+++ b/assignments/assign3/params_assign3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/assignments/assign3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="500" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00864DA7-E1F3-5148-8FBF-768C5E08D59E}"/>
+  <xr:revisionPtr revIDLastSave="501" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4FF08FB-E9BC-774E-8869-973D68F77761}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
+    <workbookView xWindow="4800" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="SCANDAT_death_multipliers" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$E$49</definedName>
     <definedName name="num_components">#REF!</definedName>
     <definedName name="PRT_cost">#REF!</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="95">
   <si>
     <t>Category</t>
   </si>
@@ -165,18 +165,6 @@
   </si>
   <si>
     <t>costFluR</t>
-  </si>
-  <si>
-    <t>False positive test result</t>
-  </si>
-  <si>
-    <t>costFP</t>
-  </si>
-  <si>
-    <t>True positive test result</t>
-  </si>
-  <si>
-    <t>costTP</t>
   </si>
   <si>
     <t>Stillbirth after congenital transmission</t>
@@ -367,6 +355,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -452,6 +441,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,11 +747,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -774,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -791,10 +784,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1">
         <v>0.95</v>
@@ -808,10 +801,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D3" s="8">
         <v>0.5</v>
@@ -825,10 +818,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D4" s="8">
         <v>0.5</v>
@@ -842,10 +835,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D5" s="8">
         <v>0.9</v>
@@ -859,10 +852,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2">
         <v>0.18360000000000001</v>
@@ -879,7 +872,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2">
         <v>0.01</v>
@@ -896,7 +889,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2">
         <v>2.58E-2</v>
@@ -913,7 +906,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -930,7 +923,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2">
         <v>4.8399999999999999E-2</v>
@@ -947,7 +940,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3">
         <v>0.121</v>
@@ -964,7 +957,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3">
         <v>0.22</v>
@@ -981,7 +974,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3">
         <v>0.48799999999999999</v>
@@ -998,7 +991,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2">
         <v>0.1</v>
@@ -1012,10 +1005,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2">
         <v>0.4</v>
@@ -1165,10 +1158,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D24" s="8">
         <v>18</v>
@@ -1182,13 +1175,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2">
-        <v>91.8</v>
+        <v>1357.8191999999999</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
@@ -1199,13 +1192,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D26" s="2">
-        <v>91.8</v>
+        <v>61675.56</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
@@ -1216,13 +1209,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2">
-        <v>1357.8191999999999</v>
+        <v>38579.576399999998</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -1233,13 +1226,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2">
-        <v>61675.56</v>
+        <v>72475.56</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -1250,13 +1243,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="D29" s="2">
-        <v>38579.576399999998</v>
+        <v>25386.371999999999</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
@@ -1267,13 +1260,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2">
-        <v>72475.56</v>
+        <v>242.78399999999999</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
@@ -1284,13 +1277,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="D31" s="2">
-        <v>25386.371999999999</v>
+        <v>505.00799999999998</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -1301,13 +1294,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D32" s="2">
-        <v>242.78399999999999</v>
+        <v>6644.808</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
@@ -1318,13 +1311,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D33" s="2">
-        <v>505.00799999999998</v>
+        <v>26131.788</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
@@ -1335,13 +1328,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D34" s="2">
-        <v>6644.808</v>
+        <v>4358764.0080000004</v>
       </c>
       <c r="E34" s="2">
         <v>0</v>
@@ -1349,16 +1342,16 @@
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="D35" s="2">
-        <v>26131.788</v>
+        <v>0.9</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
@@ -1366,16 +1359,16 @@
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2">
-        <v>4358764.0080000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
@@ -1386,16 +1379,16 @@
         <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.9</v>
+        <v>20</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.57999999999999996</v>
       </c>
       <c r="E37" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1408,11 +1401,11 @@
       <c r="C38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.56999999999999995</v>
+      <c r="D38" s="3">
+        <v>0.63</v>
       </c>
       <c r="E38" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1426,10 +1419,10 @@
         <v>20</v>
       </c>
       <c r="D39" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="E39" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1443,10 +1436,10 @@
         <v>20</v>
       </c>
       <c r="D40" s="3">
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="E40" s="2">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1454,16 +1447,16 @@
         <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="3">
-        <v>0.61</v>
+        <v>18</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.5</v>
       </c>
       <c r="E41" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1471,16 +1464,16 @@
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="E42" s="2">
         <v>20</v>
-      </c>
-      <c r="D42" s="3">
-        <v>0.59</v>
-      </c>
-      <c r="E42" s="2">
-        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1494,10 +1487,10 @@
         <v>18</v>
       </c>
       <c r="D43" s="2">
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E43" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1510,11 +1503,11 @@
       <c r="C44" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.59</v>
+      <c r="D44" s="3">
+        <v>0.55000000000000004</v>
       </c>
       <c r="E44" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1527,11 +1520,11 @@
       <c r="C45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="2">
-        <v>0.57999999999999996</v>
+      <c r="D45" s="3">
+        <v>0.54</v>
       </c>
       <c r="E45" s="2">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1539,16 +1532,16 @@
         <v>11</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="3">
-        <v>0.55000000000000004</v>
+        <v>13</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.4</v>
       </c>
       <c r="E46" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1556,30 +1549,30 @@
         <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="3">
-        <v>0.54</v>
+        <v>54</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
       </c>
       <c r="E47" s="2">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D48" s="2">
-        <v>0.4</v>
+        <v>21</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
@@ -1587,57 +1580,23 @@
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D49" s="2">
-        <v>0</v>
+        <v>79.8</v>
       </c>
       <c r="E49" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="2">
-        <v>21</v>
-      </c>
-      <c r="E50" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="2">
-        <v>79.8</v>
-      </c>
-      <c r="E51" s="2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E51" xr:uid="{0DE5FD20-882A-DF4F-9D27-F4C1D8DF0B29}"/>
+  <autoFilter ref="A1:E49" xr:uid="{0DE5FD20-882A-DF4F-9D27-F4C1D8DF0B29}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1664,10 +1623,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1675,10 +1634,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D2" s="8">
         <v>10</v>
@@ -1689,10 +1648,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D3" s="8">
         <v>6</v>
@@ -1703,10 +1662,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D4" s="8">
         <v>0.999</v>
@@ -1717,10 +1676,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D5" s="8">
         <v>0.98</v>
@@ -1731,10 +1690,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D6" s="8">
         <v>0.99970000000000003</v>
@@ -1745,10 +1704,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D7" s="8">
         <v>0.99999999900000003</v>
@@ -1759,10 +1718,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D8" s="8">
         <v>0.94399999999999995</v>
@@ -1773,10 +1732,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D9" s="8">
         <v>1.4999999999999999E-2</v>
@@ -1787,10 +1746,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D10" s="8">
         <v>0.54100000000000004</v>
@@ -1801,10 +1760,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D11" s="8">
         <v>0.5</v>
@@ -1815,10 +1774,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D12" s="8">
         <v>0.5</v>
@@ -1829,10 +1788,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" s="8">
         <v>0.9</v>
@@ -1859,7 +1818,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -2047,10 +2006,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2881,16 +2840,16 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed errors with session 11 slides and assignment 3
</commit_message>
<xml_diff>
--- a/assignments/assign3/params_assign3.xlsx
+++ b/assignments/assign3/params_assign3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/assignments/assign3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epib-676/assignments/assign3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="501" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4FF08FB-E9BC-774E-8869-973D68F77761}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCA03153-70EB-8A40-A5F5-E419B26A1BD0}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="SCANDAT_death_multipliers" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$E$47</definedName>
     <definedName name="num_components">#REF!</definedName>
     <definedName name="PRT_cost">#REF!</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="91">
   <si>
     <t>Category</t>
   </si>
@@ -126,18 +126,6 @@
   </si>
   <si>
     <t>costStillBirth</t>
-  </si>
-  <si>
-    <t>Mother testing</t>
-  </si>
-  <si>
-    <t>costMotherZikaTest</t>
-  </si>
-  <si>
-    <t>Infant testing</t>
-  </si>
-  <si>
-    <t>costInfantZikaTest</t>
   </si>
   <si>
     <t>Normal delivery</t>
@@ -747,11 +735,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -767,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -784,10 +772,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1">
         <v>0.95</v>
@@ -801,10 +789,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D3" s="8">
         <v>0.5</v>
@@ -818,10 +806,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D4" s="8">
         <v>0.5</v>
@@ -835,10 +823,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8">
         <v>0.9</v>
@@ -852,10 +840,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2">
         <v>0.18360000000000001</v>
@@ -869,10 +857,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2">
         <v>0.01</v>
@@ -886,10 +874,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2">
         <v>2.58E-2</v>
@@ -903,10 +891,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -920,10 +908,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2">
         <v>4.8399999999999999E-2</v>
@@ -937,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3">
         <v>0.121</v>
@@ -954,10 +942,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3">
         <v>0.22</v>
@@ -971,10 +959,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3">
         <v>0.48799999999999999</v>
@@ -991,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2">
         <v>0.1</v>
@@ -1005,10 +993,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2">
         <v>0.4</v>
@@ -1158,10 +1146,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D24" s="8">
         <v>18</v>
@@ -1175,10 +1163,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D25" s="2">
         <v>1357.8191999999999</v>
@@ -1192,10 +1180,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D26" s="2">
         <v>61675.56</v>
@@ -1209,10 +1197,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D27" s="2">
         <v>38579.576399999998</v>
@@ -1226,10 +1214,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2">
         <v>72475.56</v>
@@ -1243,10 +1231,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2">
         <v>25386.371999999999</v>
@@ -1260,13 +1248,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D30" s="2">
-        <v>242.78399999999999</v>
+        <v>6644.808</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
@@ -1277,13 +1265,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D31" s="2">
-        <v>505.00799999999998</v>
+        <v>26131.788</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -1294,13 +1282,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="D32" s="2">
-        <v>6644.808</v>
+        <v>4358764.0080000004</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
@@ -1308,16 +1296,16 @@
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="D33" s="2">
-        <v>26131.788</v>
+        <v>0.9</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
@@ -1325,16 +1313,16 @@
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2">
-        <v>4358764.0080000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E34" s="2">
         <v>0</v>
@@ -1345,16 +1333,16 @@
         <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.9</v>
+        <v>20</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.57999999999999996</v>
       </c>
       <c r="E35" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1367,11 +1355,11 @@
       <c r="C36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="2">
-        <v>0.56999999999999995</v>
+      <c r="D36" s="3">
+        <v>0.63</v>
       </c>
       <c r="E36" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1385,10 +1373,10 @@
         <v>20</v>
       </c>
       <c r="D37" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="E37" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1402,10 +1390,10 @@
         <v>20</v>
       </c>
       <c r="D38" s="3">
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="E38" s="2">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1413,16 +1401,16 @@
         <v>11</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0.61</v>
+        <v>18</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.5</v>
       </c>
       <c r="E39" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1430,16 +1418,16 @@
         <v>11</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="E40" s="2">
         <v>20</v>
-      </c>
-      <c r="D40" s="3">
-        <v>0.59</v>
-      </c>
-      <c r="E40" s="2">
-        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1453,10 +1441,10 @@
         <v>18</v>
       </c>
       <c r="D41" s="2">
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E41" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1469,11 +1457,11 @@
       <c r="C42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.59</v>
+      <c r="D42" s="3">
+        <v>0.55000000000000004</v>
       </c>
       <c r="E42" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1486,11 +1474,11 @@
       <c r="C43" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="2">
-        <v>0.57999999999999996</v>
+      <c r="D43" s="3">
+        <v>0.54</v>
       </c>
       <c r="E43" s="2">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1498,16 +1486,16 @@
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0.55000000000000004</v>
+        <v>13</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.4</v>
       </c>
       <c r="E44" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1515,30 +1503,30 @@
         <v>11</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0.54</v>
+        <v>50</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
       </c>
       <c r="E45" s="2">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D46" s="2">
-        <v>0.4</v>
+        <v>21</v>
       </c>
       <c r="E46" s="2">
         <v>0</v>
@@ -1546,57 +1534,23 @@
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="D47" s="2">
-        <v>0</v>
+        <v>79.8</v>
       </c>
       <c r="E47" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="2">
-        <v>21</v>
-      </c>
-      <c r="E48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="2">
-        <v>79.8</v>
-      </c>
-      <c r="E49" s="2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E49" xr:uid="{0DE5FD20-882A-DF4F-9D27-F4C1D8DF0B29}"/>
+  <autoFilter ref="A1:E47" xr:uid="{0DE5FD20-882A-DF4F-9D27-F4C1D8DF0B29}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1623,10 +1577,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1634,10 +1588,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8">
         <v>10</v>
@@ -1648,10 +1602,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" s="8">
         <v>6</v>
@@ -1662,10 +1616,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D4" s="8">
         <v>0.999</v>
@@ -1676,10 +1630,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="8">
         <v>0.98</v>
@@ -1690,10 +1644,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D6" s="8">
         <v>0.99970000000000003</v>
@@ -1704,10 +1658,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" s="8">
         <v>0.99999999900000003</v>
@@ -1718,10 +1672,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8">
         <v>0.94399999999999995</v>
@@ -1732,10 +1686,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D9" s="8">
         <v>1.4999999999999999E-2</v>
@@ -1746,10 +1700,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D10" s="8">
         <v>0.54100000000000004</v>
@@ -1760,10 +1714,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D11" s="8">
         <v>0.5</v>
@@ -1774,10 +1728,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D12" s="8">
         <v>0.5</v>
@@ -1788,10 +1742,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8">
         <v>0.9</v>
@@ -1818,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -2006,10 +1960,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2840,16 +2794,16 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>